<commit_message>
Updated `Manual_Comparison.xlsx` and combined analysis files for better reporting.
</commit_message>
<xml_diff>
--- a/Manual_Comparison.xlsx
+++ b/Manual_Comparison.xlsx
@@ -1,31 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samso\Documents\Programming\AI_flaky_test\AI_flaky_test_detection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samso\Documents\Programming\FT\AI_flaky_test_detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202D443E-0B43-4C61-A0B7-EE114F368C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F85508-6470-4EBC-96C7-3CBCA8E87257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="20055" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GEMINI 2.5 Flash TEST 00" sheetId="1" r:id="rId1"/>
+    <sheet name="PYTHON" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="158">
   <si>
     <t xml:space="preserve">Test Case </t>
-  </si>
-  <si>
-    <t>Category</t>
   </si>
   <si>
     <t>Dev Fix</t>
@@ -709,6 +707,9 @@
   </si>
   <si>
     <t>Success %</t>
+  </si>
+  <si>
+    <t>Flakiness Category</t>
   </si>
 </sst>
 </file>
@@ -1259,15 +1260,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1279,6 +1271,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1292,7 +1293,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1999,9 +2000,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BS999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomLeft" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2025,119 +2026,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="84" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="87" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="88" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E1" s="89"/>
       <c r="F1" s="89"/>
       <c r="G1" s="90"/>
       <c r="H1" s="88" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I1" s="90"/>
-      <c r="J1" s="81" t="s">
-        <v>3</v>
+      <c r="J1" s="85" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="86"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
       <c r="D2" s="91"/>
       <c r="E2" s="92"/>
       <c r="F2" s="92"/>
       <c r="G2" s="93"/>
       <c r="H2" s="91"/>
       <c r="I2" s="93"/>
-      <c r="J2" s="82"/>
+      <c r="J2" s="86"/>
     </row>
     <row r="3" spans="1:71" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
+      <c r="A3" s="83"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
       <c r="D3" s="94"/>
       <c r="E3" s="95"/>
       <c r="F3" s="95"/>
       <c r="G3" s="96"/>
       <c r="H3" s="94"/>
       <c r="I3" s="96"/>
-      <c r="J3" s="82"/>
+      <c r="J3" s="86"/>
     </row>
     <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86"/>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87" t="s">
+      <c r="A4" s="83"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="87"/>
-      <c r="J4" s="83"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="84"/>
+      <c r="J4" s="87"/>
       <c r="O4" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="P4" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="P4" s="58" t="s">
+      <c r="Q4" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="Q4" s="58" t="s">
-        <v>124</v>
-      </c>
       <c r="R4" s="76" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:71" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="D5" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="F5" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="J5" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="84" t="s">
-        <v>133</v>
+      <c r="M5" s="81" t="s">
+        <v>132</v>
       </c>
       <c r="N5" s="59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O5" s="59">
         <f>COUNTIF(D5:D20,D20)</f>
@@ -2158,40 +2159,40 @@
     </row>
     <row r="6" spans="1:71" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="D6" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="65" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="34" t="s">
+      <c r="F6" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="61" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="34" t="s">
+      <c r="H6" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" s="34" t="s">
         <v>23</v>
-      </c>
-      <c r="H6" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="J6" s="34" t="s">
-        <v>24</v>
       </c>
       <c r="K6" s="32"/>
       <c r="L6" s="32"/>
-      <c r="M6" s="85"/>
+      <c r="M6" s="82"/>
       <c r="N6" s="59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O6" s="59">
         <f>COUNTIF(F5:F20,D20)</f>
@@ -2218,42 +2219,42 @@
     </row>
     <row r="7" spans="1:71" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="37" t="s">
+      <c r="D7" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="34" t="s">
+      <c r="F7" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="34" t="s">
+      <c r="H7" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" s="37" t="s">
         <v>28</v>
-      </c>
-      <c r="H7" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="J7" s="37" t="s">
-        <v>29</v>
       </c>
       <c r="K7" s="33"/>
       <c r="L7" s="33"/>
       <c r="M7" s="59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N7" s="59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O7" s="59">
         <f>COUNTIF(H5:H20,D5)</f>
@@ -2280,34 +2281,34 @@
     </row>
     <row r="8" spans="1:71" s="41" customFormat="1" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="38" t="s">
+      <c r="D8" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="66" t="s">
+      <c r="F8" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" s="38" t="s">
         <v>34</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="62" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="73" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="J8" s="38" t="s">
-        <v>35</v>
       </c>
       <c r="K8"/>
       <c r="L8"/>
@@ -2373,34 +2374,34 @@
     </row>
     <row r="9" spans="1:71" s="41" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="38" t="s">
+      <c r="D9" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="64" t="s">
-        <v>137</v>
-      </c>
-      <c r="E9" s="34" t="s">
+      <c r="F9" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>39</v>
-      </c>
       <c r="H9" s="73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J9" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K9" s="32"/>
       <c r="L9" s="32"/>
@@ -2466,34 +2467,34 @@
     </row>
     <row r="10" spans="1:71" s="42" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="37" t="s">
+      <c r="D10" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="67" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="34" t="s">
+      <c r="F10" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="34" t="s">
+      <c r="H10" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="J10" s="37" t="s">
         <v>43</v>
-      </c>
-      <c r="H10" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="J10" s="37" t="s">
-        <v>44</v>
       </c>
       <c r="K10" s="32"/>
       <c r="L10" s="32"/>
@@ -2559,34 +2560,34 @@
     </row>
     <row r="11" spans="1:71" s="42" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="C11" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="D11" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="34" t="s">
+      <c r="F11" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="34" t="s">
+      <c r="H11" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" s="37" t="s">
         <v>49</v>
-      </c>
-      <c r="H11" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="J11" s="37" t="s">
-        <v>50</v>
       </c>
       <c r="K11"/>
       <c r="L11"/>
@@ -2652,34 +2653,34 @@
     </row>
     <row r="12" spans="1:71" s="47" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="45" t="s">
+      <c r="D12" s="68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="68" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="46" t="s">
+      <c r="F12" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="70" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="46" t="s">
+      <c r="H12" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="J12" s="43" t="s">
         <v>54</v>
-      </c>
-      <c r="H12" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="J12" s="43" t="s">
-        <v>55</v>
       </c>
       <c r="K12"/>
       <c r="L12"/>
@@ -2745,34 +2746,34 @@
     </row>
     <row r="13" spans="1:71" s="42" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="37" t="s">
+      <c r="D13" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="34" t="s">
+      <c r="F13" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="J13" s="37" t="s">
         <v>58</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="J13" s="37" t="s">
-        <v>59</v>
       </c>
       <c r="K13"/>
       <c r="L13"/>
@@ -2838,226 +2839,226 @@
     </row>
     <row r="14" spans="1:71" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="C14" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="D14" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="34" t="s">
+      <c r="F14" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="34" t="s">
+      <c r="H14" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14" s="37" t="s">
         <v>69</v>
-      </c>
-      <c r="H14" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="37" t="s">
-        <v>141</v>
-      </c>
-      <c r="J14" s="37" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:71" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="37" t="s">
+      <c r="D15" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="34" t="s">
+      <c r="F15" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="34" t="s">
+      <c r="H15" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="J15" s="37" t="s">
         <v>74</v>
-      </c>
-      <c r="H15" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I15" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="J15" s="37" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:71" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="C16" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="36" t="s">
+      <c r="D16" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="34" t="s">
+      <c r="F16" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="F16" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="34" t="s">
+      <c r="H16" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="J16" s="37" t="s">
         <v>80</v>
-      </c>
-      <c r="H16" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="37" t="s">
-        <v>143</v>
-      </c>
-      <c r="J16" s="37" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:71" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="C17" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="D17" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="34" t="s">
+      <c r="F17" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="34" t="s">
+      <c r="H17" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" s="37" t="s">
         <v>92</v>
-      </c>
-      <c r="H17" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="37" t="s">
-        <v>144</v>
-      </c>
-      <c r="J17" s="37" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:71" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="37" t="s">
+      <c r="D18" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="34" t="s">
+      <c r="F18" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="34" t="s">
+      <c r="H18" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="J18" s="37" t="s">
         <v>97</v>
-      </c>
-      <c r="H18" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="37" t="s">
-        <v>145</v>
-      </c>
-      <c r="J18" s="37" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:71" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="37" t="s">
+      <c r="D19" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="D19" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="34" t="s">
+      <c r="F19" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="34" t="s">
+      <c r="H19" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="J19" s="37" t="s">
         <v>107</v>
-      </c>
-      <c r="H19" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="J19" s="37" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:71" s="42" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="B20" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="55" t="s">
+      <c r="D20" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="D20" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="57" t="s">
+      <c r="F20" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="F20" s="71" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="57" t="s">
+      <c r="H20" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="J20" s="55" t="s">
         <v>116</v>
-      </c>
-      <c r="H20" s="75" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="55" t="s">
-        <v>149</v>
-      </c>
-      <c r="J20" s="55" t="s">
-        <v>117</v>
       </c>
       <c r="K20"/>
       <c r="L20"/>
@@ -3171,192 +3172,192 @@
     </row>
     <row r="26" spans="1:71" s="7" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="C26" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>120</v>
-      </c>
       <c r="D26" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="19"/>
       <c r="J26" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:71" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="10" t="s">
+      <c r="D27" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="13" t="s">
+      <c r="F27" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="16"/>
       <c r="J27" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:71" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="D28" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>101</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>102</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="16"/>
       <c r="J28" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K28" s="78" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:71" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="10" t="s">
+      <c r="D29" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="13" t="s">
+      <c r="F29" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="12" t="s">
         <v>62</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>63</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="16"/>
       <c r="J29" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K29" s="78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:71" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="8" t="s">
+      <c r="F30" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="15"/>
       <c r="J30" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K30" s="79" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:71" s="54" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" s="48" t="s">
+      <c r="D31" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="51" t="s">
+      <c r="F31" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="H31" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="J31" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F31" s="52" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="51" t="s">
-        <v>147</v>
-      </c>
-      <c r="H31" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="I31" s="48" t="s">
-        <v>148</v>
-      </c>
-      <c r="J31" s="48" t="s">
-        <v>112</v>
-      </c>
       <c r="K31" s="80" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:71" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -14981,4 +14982,612 @@
   <pageSetup orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D736104C-1C3C-4BB6-87B4-AD8C3115F3A1}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="10" max="10" width="35.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="84" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="88" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="88" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="90"/>
+      <c r="J1" s="85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="86"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="83"/>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="86"/>
+    </row>
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="83"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="84"/>
+      <c r="J4" s="87"/>
+    </row>
+    <row r="5" spans="1:10" ht="390.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="J10" s="37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="J11" s="37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="270.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="J12" s="43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="J13" s="37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="J15" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="J16" s="37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="J19" s="37" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="375" x14ac:dyDescent="0.3">
+      <c r="A20" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="71" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="J20" s="55" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:G3"/>
+    <mergeCell ref="H1:I3"/>
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>